<commit_message>
mysql load data done
</commit_message>
<xml_diff>
--- a/xls/schema/mysql/gameAdmin1.xlsx
+++ b/xls/schema/mysql/gameAdmin1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
   <si>
     <t>PartitionBy</t>
   </si>
@@ -277,9 +277,6 @@
     <t>日期</t>
   </si>
   <si>
-    <t>日期2</t>
-  </si>
-  <si>
     <t>ID</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -368,9 +365,6 @@
   </si>
   <si>
     <t>Area</t>
-  </si>
-  <si>
-    <t>time33</t>
   </si>
 </sst>
 </file>
@@ -983,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N24" sqref="A5:N24"/>
     </sheetView>
   </sheetViews>
@@ -991,25 +985,25 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="12">
       <c r="A1" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>82</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>6</v>
@@ -1018,13 +1012,13 @@
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -1035,13 +1029,13 @@
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A3" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -1052,13 +1046,13 @@
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A4" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -1304,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1371,7 +1365,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>9</v>
@@ -1506,20 +1500,6 @@
       </c>
       <c r="F12" s="8" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1546,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -1584,10 +1564,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>9</v>
@@ -1600,7 +1580,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>23</v>
@@ -1611,12 +1591,12 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>23</v>
@@ -1627,12 +1607,12 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>23</v>
@@ -1643,12 +1623,12 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
@@ -1659,15 +1639,15 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -1675,15 +1655,15 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -1691,15 +1671,15 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -1707,7 +1687,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>